<commit_message>
14.01.2025: commit after BJMS review
</commit_message>
<xml_diff>
--- a/res/0724_yves_complex/multivariate_GEE.xlsx
+++ b/res/0724_yves_complex/multivariate_GEE.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13130" windowHeight="6110" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13130" windowHeight="6110"/>
   </bookViews>
   <sheets>
-    <sheet name="n=500_sc=1" sheetId="2" r:id="rId1"/>
-    <sheet name="n=500_sc=2" sheetId="3" r:id="rId2"/>
-    <sheet name="n=500_sc=4" sheetId="4" r:id="rId3"/>
-    <sheet name="n=1000_sc=1" sheetId="5" r:id="rId4"/>
-    <sheet name="n=1000_sc=2" sheetId="6" r:id="rId5"/>
-    <sheet name="n=1000_sc=4" sheetId="7" r:id="rId6"/>
+    <sheet name="GEE performance" sheetId="8" r:id="rId1"/>
+    <sheet name="n=500_sc=1" sheetId="2" r:id="rId2"/>
+    <sheet name="n=500_sc=2" sheetId="3" r:id="rId3"/>
+    <sheet name="n=500_sc=4" sheetId="4" r:id="rId4"/>
+    <sheet name="n=1000_sc=1" sheetId="5" r:id="rId5"/>
+    <sheet name="n=1000_sc=2" sheetId="6" r:id="rId6"/>
+    <sheet name="n=1000_sc=4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="23">
   <si>
     <t/>
   </si>
@@ -71,6 +72,33 @@
   </si>
   <si>
     <t>GEE</t>
+  </si>
+  <si>
+    <t>Type I Error</t>
+  </si>
+  <si>
+    <t>Power (only $\boldymbol{\lambda}$-fluctuation )</t>
+  </si>
+  <si>
+    <t>n=500, l=2</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>CvM</t>
+  </si>
+  <si>
+    <t>maxLM</t>
+  </si>
+  <si>
+    <t>maxLMo</t>
+  </si>
+  <si>
+    <t>WDMo</t>
+  </si>
+  <si>
+    <t>LMuo</t>
   </si>
 </sst>
 </file>
@@ -120,11 +148,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -410,10 +443,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3.4387900000000027E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.9889135254988899E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.3245383</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.67724867724867699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3.0261300000000046E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.2106430155210597E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.43139840000000002</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.59656084656084696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.7510299999999988E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.43458980044346E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.39577839999999997</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.63095238095238104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3.5763400000000001E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.2106430155210597E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.4208443</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.60185185185185197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5.9147199999999955E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5.9866962305986697E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.31926120000000002</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.70767195767195801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2.475930000000004E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.9889135254988899E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.35224270000000002</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.66269841269841301</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +732,124 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.9767441860465018E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.69767441860465107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.31395348837209303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.60465116279069808</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.24418604651162801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5.8139534883721034E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>11.064232842866801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>12.8700645635294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>10.636003488718099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.97499999999999898</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -574,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>6.9767441860465018E-2</v>
+        <v>0.10526315789473695</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -582,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.69767441860465107</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -590,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.31395348837209303</v>
+        <v>0.81052631578947398</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -598,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.60465116279069808</v>
+        <v>0.61052631578947403</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.24418604651162801</v>
+        <v>0.326315789473684</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>5.8139534883721034E-2</v>
+        <v>0.115789473684211</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,7 +933,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>11.064232842866801</v>
+        <v>28.273513558036399</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -638,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>12.8700645635294</v>
+        <v>34.000978745912199</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -646,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>10.636003488718099</v>
+        <v>31.233495478881</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -654,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>0.97499999999999898</v>
+        <v>1.35452631578947</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +966,145 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.7777777777777946E-2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3.0567699999999975E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.18888888888888899</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.72926E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.18888888888888899</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.6026200000000008E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.344444444444444</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.8034899999999991E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.23333333333333295</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.6943199999999963E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5.5555555555556024E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.6200899999999971E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>6.1997634384367197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>6.5762863900926396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>5.8313169982698199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.91810000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -691,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.10526315789473695</v>
+        <v>9.1836734693877986E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -699,7 +1140,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0.530612244897959</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -707,7 +1148,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.81052631578947398</v>
+        <v>0.22448979591836704</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -715,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.61052631578947403</v>
+        <v>0.33673469387755095</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -723,7 +1164,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.326315789473684</v>
+        <v>0.19387755102040805</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -731,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>0.115789473684211</v>
+        <v>5.102040816326503E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -747,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>28.273513558036399</v>
+        <v>11.0913479960695</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -755,7 +1196,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>34.000978745912199</v>
+        <v>12.233323904932799</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -763,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>31.233495478881</v>
+        <v>10.9827486617225</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -771,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>1.35452631578947</v>
+        <v>1.0219591836734701</v>
       </c>
     </row>
   </sheetData>
@@ -780,262 +1221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>7.7777777777777946E-2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3.0567699999999975E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.18888888888888899</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2.72926E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.18888888888888899</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3.6026200000000008E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.344444444444444</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4.8034899999999991E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.23333333333333295</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4.6943199999999963E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5.5555555555556024E-2</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2.6200899999999971E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>6.1997634384367197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>6.5762863900926396</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>5.8313169982698199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>0.91810000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>9.1836734693877986E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.530612244897959</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.22448979591836704</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.33673469387755095</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.19387755102040805</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5.102040816326503E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>11.0913479960695</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>12.233323904932799</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>10.9827486617225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>1.0219591836734701</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>

</xml_diff>